<commit_message>
added an IHU requirement
</commit_message>
<xml_diff>
--- a/CougSat1/CougSat1-SystemRequirements.xlsx
+++ b/CougSat1/CougSat1-SystemRequirements.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Bradley\Documents\CougsInSpace\CougSat1-Hardware\CougSat1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cody\Documents\CiS\HardwareRepo\CougSat1-Hardware\CougSat1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2978F82D-8C43-4D91-8975-B4F526C97189}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{CB9DAC32-F6C0-4444-9FE8-EF92C5E1C529}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7548"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="192">
   <si>
     <t>CougSat-1 System Requirements</t>
   </si>
@@ -592,12 +591,21 @@
   </si>
   <si>
     <t>REQ-075</t>
+  </si>
+  <si>
+    <t>REQ-076</t>
+  </si>
+  <si>
+    <t>The IHU shall operate as a RTOS.</t>
+  </si>
+  <si>
+    <t>Need to process mission critical events as they happen.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -973,24 +981,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44F803DB-0F99-4F01-884A-5A7CE521278A}">
-  <dimension ref="A1:G78"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C79" sqref="C79"/>
+      <pane ySplit="3" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="2" max="2" width="72.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="50.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" customWidth="1"/>
+    <col min="2" max="2" width="72.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="50.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1001,7 +1009,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
@@ -1012,7 +1020,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -1029,7 +1037,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1046,7 +1054,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1063,7 +1071,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>36</v>
       </c>
@@ -1080,7 +1088,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
@@ -1097,7 +1105,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>38</v>
       </c>
@@ -1114,7 +1122,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>39</v>
       </c>
@@ -1131,7 +1139,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>40</v>
       </c>
@@ -1148,7 +1156,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>41</v>
       </c>
@@ -1165,7 +1173,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>42</v>
       </c>
@@ -1182,7 +1190,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>43</v>
       </c>
@@ -1199,7 +1207,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>44</v>
       </c>
@@ -1216,7 +1224,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
@@ -1233,7 +1241,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -1250,7 +1258,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
@@ -1267,7 +1275,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>48</v>
       </c>
@@ -1284,7 +1292,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>49</v>
       </c>
@@ -1301,7 +1309,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>50</v>
       </c>
@@ -1318,7 +1326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>51</v>
       </c>
@@ -1335,7 +1343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>52</v>
       </c>
@@ -1352,7 +1360,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>53</v>
       </c>
@@ -1369,7 +1377,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>54</v>
       </c>
@@ -1386,7 +1394,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>55</v>
       </c>
@@ -1403,7 +1411,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>56</v>
       </c>
@@ -1420,7 +1428,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>57</v>
       </c>
@@ -1437,7 +1445,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>58</v>
       </c>
@@ -1454,7 +1462,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>59</v>
       </c>
@@ -1471,7 +1479,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>60</v>
       </c>
@@ -1488,7 +1496,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>61</v>
       </c>
@@ -1505,7 +1513,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
@@ -1522,7 +1530,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>63</v>
       </c>
@@ -1539,7 +1547,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>64</v>
       </c>
@@ -1556,7 +1564,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>65</v>
       </c>
@@ -1573,7 +1581,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>66</v>
       </c>
@@ -1590,7 +1598,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>67</v>
       </c>
@@ -1607,7 +1615,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>68</v>
       </c>
@@ -1624,7 +1632,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>69</v>
       </c>
@@ -1641,7 +1649,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>70</v>
       </c>
@@ -1658,7 +1666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>71</v>
       </c>
@@ -1675,7 +1683,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>72</v>
       </c>
@@ -1692,7 +1700,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>73</v>
       </c>
@@ -1709,7 +1717,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>74</v>
       </c>
@@ -1726,7 +1734,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>75</v>
       </c>
@@ -1743,7 +1751,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>76</v>
       </c>
@@ -1760,7 +1768,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>77</v>
       </c>
@@ -1777,7 +1785,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>78</v>
       </c>
@@ -1794,7 +1802,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>117</v>
       </c>
@@ -1811,7 +1819,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>118</v>
       </c>
@@ -1828,7 +1836,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>119</v>
       </c>
@@ -1845,7 +1853,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>120</v>
       </c>
@@ -1862,7 +1870,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>121</v>
       </c>
@@ -1879,7 +1887,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>122</v>
       </c>
@@ -1896,7 +1904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>123</v>
       </c>
@@ -1913,7 +1921,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>124</v>
       </c>
@@ -1930,7 +1938,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>125</v>
       </c>
@@ -1947,7 +1955,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>126</v>
       </c>
@@ -1964,32 +1972,32 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>103</v>
+        <v>190</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="D59" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="E59" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>128</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
       <c r="D60" t="s">
         <v>11</v>
@@ -1998,15 +2006,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>129</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D61" t="s">
         <v>11</v>
@@ -2015,15 +2023,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>130</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D62" t="s">
         <v>11</v>
@@ -2032,15 +2040,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>131</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D63" t="s">
         <v>11</v>
@@ -2049,15 +2057,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>132</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>170</v>
+        <v>107</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D64" t="s">
         <v>11</v>
@@ -2066,46 +2074,46 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D65" t="s">
-        <v>93</v>
+        <v>11</v>
       </c>
       <c r="E65" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>134</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D66" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="E66" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>135</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>174</v>
@@ -2117,15 +2125,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>136</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>175</v>
+        <v>109</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D68" t="s">
         <v>11</v>
@@ -2134,66 +2142,66 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>116</v>
+        <v>175</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="D69" t="s">
-        <v>110</v>
+        <v>11</v>
       </c>
       <c r="E69" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>138</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="D70" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E70" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="D71" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E71" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>140</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>112</v>
+        <v>155</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D72" t="s">
         <v>110</v>
@@ -2202,15 +2210,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D73" t="s">
         <v>110</v>
@@ -2219,15 +2227,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D74" t="s">
         <v>110</v>
@@ -2236,71 +2244,88 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>144</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>146</v>
+        <v>115</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D75" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E75" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>145</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D76" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="E76" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>184</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D77" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="E77" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>188</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D78" t="s">
         <v>111</v>
       </c>
       <c r="E78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D79" t="s">
+        <v>111</v>
+      </c>
+      <c r="E79" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>